<commit_message>
excel feito e adicionado grafico no word
</commit_message>
<xml_diff>
--- a/proj2/Book1.xlsx
+++ b/proj2/Book1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">teste</t>
   </si>
@@ -31,22 +31,19 @@
     <t xml:space="preserve">entradas diferentes de 0</t>
   </si>
   <si>
-    <t xml:space="preserve">max cost of any process execution</t>
+    <t xml:space="preserve">max cost of any process execution (irrelevante)</t>
   </si>
   <si>
     <t xml:space="preserve">Vertices = processos + 2</t>
   </si>
   <si>
-    <t xml:space="preserve">Edges = processos*2 + n de entradas diferentes de 0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V+E</t>
+    <t xml:space="preserve">Edges = processos*2 + n de entradas diferentes de 0 *2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V*E</t>
   </si>
   <si>
     <t xml:space="preserve">tempo de execucao(s)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dag1</t>
   </si>
   <si>
     <t xml:space="preserve">dag2</t>
@@ -83,7 +80,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -105,12 +102,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -172,7 +163,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -248,7 +239,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -341,49 +332,46 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$10</c:f>
+              <c:f>Sheet1!$G$2:$G$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>167378</c:v>
-                </c:pt>
+                <c:ptCount val="10"/>
                 <c:pt idx="1">
-                  <c:v>660450</c:v>
+                  <c:v>2628401776</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1476198</c:v>
+                  <c:v>8827032768</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2584446</c:v>
+                  <c:v>20621825760</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3991840</c:v>
+                  <c:v>39834267336</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5864766</c:v>
+                  <c:v>70256531040</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8027818</c:v>
+                  <c:v>112225423248</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10129194</c:v>
+                  <c:v>161851460752</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13087774</c:v>
+                  <c:v>235308103072</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1411702764</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$10</c:f>
+              <c:f>Sheet1!$H$2:$H$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1.385</c:v>
-                </c:pt>
+                <c:ptCount val="10"/>
                 <c:pt idx="1">
                   <c:v>13.719</c:v>
                 </c:pt>
@@ -407,17 +395,20 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1428.439</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.317</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="71836523"/>
-        <c:axId val="11835826"/>
+        <c:axId val="82873104"/>
+        <c:axId val="89013476"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71836523"/>
+        <c:axId val="82873104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -454,7 +445,8 @@
                     </a:solidFill>
                     <a:latin typeface="Calibri"/>
                   </a:rPr>
-                  <a:t>Numero de Vértices + Edges</a:t>
+                  <a:t>Numero de Vértices*Edges
+</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -493,12 +485,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11835826"/>
+        <c:crossAx val="89013476"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="11835826"/>
+        <c:axId val="89013476"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -574,7 +566,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71836523"/>
+        <c:crossAx val="82873104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -606,16 +598,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>583920</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>3240</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>146520</xdr:rowOff>
+      <xdr:rowOff>146880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>297000</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>93600</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>41760</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>190800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -623,8 +615,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11270880" y="321480"/>
-        <a:ext cx="5783760" cy="2751480"/>
+        <a:off x="9502560" y="327600"/>
+        <a:ext cx="7658640" cy="3633120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -644,21 +636,23 @@
   </sheetPr>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H:H"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N24" activeCellId="0" sqref="N24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -684,38 +678,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>164372</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <f aca="false">(B2+2)</f>
-        <v>1002</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <f aca="false">SUM(E2*2+C2)</f>
-        <v>166376</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <f aca="false">SUM(E2,F2)</f>
-        <v>167378</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>1.385</v>
-      </c>
-    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>2000</v>
@@ -731,20 +697,20 @@
         <v>2002</v>
       </c>
       <c r="F3" s="0" t="n">
-        <f aca="false">SUM(E3*2+C3)</f>
-        <v>658448</v>
+        <f aca="false">SUM(2*B3,2*C3)</f>
+        <v>1312888</v>
       </c>
       <c r="G3" s="0" t="n">
-        <f aca="false">SUM(E3,F3)</f>
-        <v>660450</v>
+        <f aca="false">E3*F3</f>
+        <v>2628401776</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>13.719</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>3000</v>
@@ -760,20 +726,20 @@
         <v>3002</v>
       </c>
       <c r="F4" s="0" t="n">
-        <f aca="false">SUM(E4*2+C4)</f>
-        <v>1473196</v>
+        <f aca="false">SUM(2*B4,2*C4)</f>
+        <v>2940384</v>
       </c>
       <c r="G4" s="0" t="n">
-        <f aca="false">SUM(E4,F4)</f>
-        <v>1476198</v>
+        <f aca="false">E4*F4</f>
+        <v>8827032768</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>49.66</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>4000</v>
@@ -789,20 +755,20 @@
         <v>4002</v>
       </c>
       <c r="F5" s="0" t="n">
-        <f aca="false">SUM(E5*2+C5)</f>
-        <v>2580444</v>
+        <f aca="false">SUM(2*B5,2*C5)</f>
+        <v>5152880</v>
       </c>
       <c r="G5" s="0" t="n">
-        <f aca="false">SUM(E5,F5)</f>
-        <v>2584446</v>
+        <f aca="false">E5*F5</f>
+        <v>20621825760</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>123.903</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>5000</v>
@@ -818,20 +784,20 @@
         <v>5002</v>
       </c>
       <c r="F6" s="0" t="n">
-        <f aca="false">SUM(E6*2+C6)</f>
-        <v>3986838</v>
+        <f aca="false">SUM(2*B6,2*C6)</f>
+        <v>7963668</v>
       </c>
       <c r="G6" s="0" t="n">
-        <f aca="false">SUM(E6,F6)</f>
-        <v>3991840</v>
+        <f aca="false">E6*F6</f>
+        <v>39834267336</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>238.594</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>6000</v>
@@ -847,20 +813,20 @@
         <v>6002</v>
       </c>
       <c r="F7" s="0" t="n">
-        <f aca="false">SUM(E7*2+C7)</f>
-        <v>5858764</v>
+        <f aca="false">SUM(2*B7,2*C7)</f>
+        <v>11705520</v>
       </c>
       <c r="G7" s="0" t="n">
-        <f aca="false">SUM(E7,F7)</f>
-        <v>5864766</v>
+        <f aca="false">E7*F7</f>
+        <v>70256531040</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>419.403</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>7000</v>
@@ -876,20 +842,20 @@
         <v>7002</v>
       </c>
       <c r="F8" s="0" t="n">
-        <f aca="false">SUM(E8*2+C8)</f>
-        <v>8020816</v>
+        <f aca="false">SUM(2*B8,2*C8)</f>
+        <v>16027624</v>
       </c>
       <c r="G8" s="0" t="n">
-        <f aca="false">SUM(E8,F8)</f>
-        <v>8027818</v>
+        <f aca="false">E8*F8</f>
+        <v>112225423248</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>672.242</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>8000</v>
@@ -905,20 +871,20 @@
         <v>8002</v>
       </c>
       <c r="F9" s="0" t="n">
-        <f aca="false">SUM(E9*2+C9)</f>
-        <v>10121192</v>
+        <f aca="false">SUM(2*B9,2*C9)</f>
+        <v>20226376</v>
       </c>
       <c r="G9" s="0" t="n">
-        <f aca="false">SUM(E9,F9)</f>
-        <v>10129194</v>
+        <f aca="false">E9*F9</f>
+        <v>161851460752</v>
       </c>
       <c r="H9" s="0" t="n">
         <v>1008.464</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>9000</v>
@@ -934,23 +900,23 @@
         <v>9002</v>
       </c>
       <c r="F10" s="0" t="n">
-        <f aca="false">SUM(E10*2+C10)</f>
-        <v>13078772</v>
+        <f aca="false">SUM(2*B10,2*C10)</f>
+        <v>26139536</v>
       </c>
       <c r="G10" s="0" t="n">
-        <f aca="false">SUM(E10,F10)</f>
-        <v>13087774</v>
+        <f aca="false">E10*F10</f>
+        <v>235308103072</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>1428.439</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>10000</v>
+        <v>1500</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>468441</v>
@@ -960,15 +926,15 @@
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">(B11+2)</f>
-        <v>10002</v>
+        <v>1502</v>
       </c>
       <c r="F11" s="0" t="n">
-        <f aca="false">SUM(E11*2+C11)</f>
-        <v>488445</v>
+        <f aca="false">SUM(2*B11,2*C11)</f>
+        <v>939882</v>
       </c>
       <c r="G11" s="0" t="n">
-        <f aca="false">SUM(E11,F11)</f>
-        <v>498447</v>
+        <f aca="false">E11*F11</f>
+        <v>1411702764</v>
       </c>
       <c r="H11" s="0" t="n">
         <v>6.317</v>

</xml_diff>